<commit_message>
Fill data mapping template
</commit_message>
<xml_diff>
--- a/data/mapping template.xlsx
+++ b/data/mapping template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="84">
   <si>
     <t xml:space="preserve">DWH table</t>
   </si>
@@ -43,54 +43,78 @@
     <t xml:space="preserve">d_antenna_sid</t>
   </si>
   <si>
+    <t xml:space="preserve">/</t>
+  </si>
+  <si>
     <t xml:space="preserve">antenna_id</t>
   </si>
   <si>
+    <t xml:space="preserve">Antenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antenna_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">antenna_radius</t>
   </si>
   <si>
-    <t xml:space="preserve">antenna_name</t>
+    <t xml:space="preserve">Radius</t>
   </si>
   <si>
     <t xml:space="preserve">antenna_capacity</t>
   </si>
   <si>
+    <t xml:space="preserve">Capacity</t>
+  </si>
+  <si>
     <t xml:space="preserve">antenna_traffic</t>
   </si>
   <si>
+    <t xml:space="preserve">MaxTraffic</t>
+  </si>
+  <si>
     <t xml:space="preserve">antenna_location_id</t>
   </si>
   <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antenna.LocationId</t>
+  </si>
+  <si>
     <t xml:space="preserve">antenna_location_x</t>
   </si>
   <si>
+    <t xml:space="preserve">PositionX</t>
+  </si>
+  <si>
     <t xml:space="preserve">antenna_location_y</t>
   </si>
   <si>
+    <t xml:space="preserve">PositionY</t>
+  </si>
+  <si>
     <t xml:space="preserve">d_customer</t>
   </si>
   <si>
     <t xml:space="preserve">d_customer_sid</t>
   </si>
   <si>
-    <t xml:space="preserve">/</t>
-  </si>
-  <si>
     <t xml:space="preserve">customer_id</t>
   </si>
   <si>
     <t xml:space="preserve">Customer</t>
   </si>
   <si>
-    <t xml:space="preserve">Id</t>
-  </si>
-  <si>
     <t xml:space="preserve">customer_name</t>
   </si>
   <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">customer_phone</t>
   </si>
   <si>
@@ -106,24 +130,15 @@
     <t xml:space="preserve">customer_location_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Location</t>
-  </si>
-  <si>
     <t xml:space="preserve">Customer.LocationId</t>
   </si>
   <si>
     <t xml:space="preserve">customer_location_x</t>
   </si>
   <si>
-    <t xml:space="preserve">PositionX</t>
-  </si>
-  <si>
     <t xml:space="preserve">customer_location_y</t>
   </si>
   <si>
-    <t xml:space="preserve">PositionY</t>
-  </si>
-  <si>
     <t xml:space="preserve">d_customer_type </t>
   </si>
   <si>
@@ -145,94 +160,118 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">d_region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d_region_sid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region_population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region_x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region_y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">positionY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_customer_activity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_customer_activity_sid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activity_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activity_traffic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activity_speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_type_sid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d_customer_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomerType.Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_sid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer.Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antenna_sid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antenna.Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region_sid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region.Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activity_date_sid</t>
+  </si>
+  <si>
     <t xml:space="preserve">d_date</t>
   </si>
   <si>
+    <t xml:space="preserve">d_date_sid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d_date.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_antenna_coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_antenna_coverage_sid</t>
+  </si>
+  <si>
     <t xml:space="preserve">date_sid</t>
   </si>
   <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quarter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weekend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d_region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d_region_sid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">region_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">region_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">region_population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">region_x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">region_y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">positionY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f_customer_activity </t>
-  </si>
-  <si>
-    <t xml:space="preserve">f_customer_activity_sid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activity_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activity_traffic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activity_speed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer_type_sid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer_sid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">antenna_sid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">region_sid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activity_date_sid</t>
+    <t xml:space="preserve">coverage_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AntennaCoverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coverage_capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coverage_traffic</t>
   </si>
 </sst>
 </file>
@@ -242,7 +281,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -264,6 +303,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -327,7 +372,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -340,8 +385,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -424,16 +477,16 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,13 +513,25 @@
       <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,7 +539,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,7 +553,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,7 +567,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -498,7 +581,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,7 +595,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,7 +612,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -522,408 +626,529 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>34</v>
+      <c r="A21" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
-        <v>34</v>
+      <c r="A22" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>34</v>
+      <c r="A23" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>34</v>
+      <c r="A24" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="0" t="s">
+      <c r="E40" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="B41" s="0" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>60</v>
+        <v>75</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="s">
-        <v>61</v>
+      <c r="A48" s="0" t="s">
+        <v>77</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="s">
-        <v>61</v>
+      <c r="A49" s="0" t="s">
+        <v>77</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
+        <v>71</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>